<commit_message>
Fix active cell issue when freezing panes
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/FreezePanes.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/FreezePanes.xlsx
@@ -6,7 +6,10 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Freeze View" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Freeze1" sheetId="2" r:id="rId2"/>
+    <x:sheet name="FreezeRows" sheetId="3" r:id="rId3"/>
+    <x:sheet name="FreezeColumns" sheetId="4" r:id="rId4"/>
+    <x:sheet name="Split View" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -363,10 +366,81 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:E5"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:pane xSplit="3" ySplit="3" topLeftCell="D4" state="frozenSplit"/>
+      <x:pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozenSplit"/>
+      <x:selection activeCell="E5" sqref="E5"/>
+      <x:selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E5"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0">
+      <x:pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
+      <x:selection activeCell="E5" sqref="E5"/>
+      <x:selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E5"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0">
+      <x:pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozenSplit"/>
+      <x:selection activeCell="E5" sqref="E5"/>
+      <x:selection pane="topRight" activeCell="E5" sqref="E5"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B2"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0">
+      <x:pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozenSplit"/>
+      <x:selection activeCell="B2" sqref="B2"/>
+      <x:selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>

</xml_diff>